<commit_message>
added the articles topicized
</commit_message>
<xml_diff>
--- a/hw8/LSA_group_3.xlsx
+++ b/hw8/LSA_group_3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Politics</t>
+          <t>Tech</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Tech</t>
+          <t>Business/Politics</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -457,11 +457,6 @@
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Science</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Business</t>
         </is>
       </c>
     </row>
@@ -491,11 +486,6 @@
           <t>sample</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>dish</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -523,11 +513,6 @@
           <t>asteroid</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>player</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -555,11 +540,6 @@
           <t>earth</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>league</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -587,11 +567,6 @@
           <t>osiris</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>golf</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -619,11 +594,6 @@
           <t>rex</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>team</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -651,11 +621,6 @@
           <t>capsule</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -683,11 +648,6 @@
           <t>dish</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>game</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -715,11 +675,6 @@
           <t>spacecraft</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>noodle</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -747,11 +702,6 @@
           <t>space</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>season</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -779,11 +729,6 @@
           <t>mission</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>pork</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -811,11 +756,6 @@
           <t>bennu</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>rice</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -843,11 +783,6 @@
           <t>pork</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>match</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -875,11 +810,6 @@
           <t>noodle</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>many</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -907,11 +837,6 @@
           <t>rice</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>year</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -939,11 +864,6 @@
           <t>system</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>one</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -971,11 +891,6 @@
           <t>chinese</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>sauce</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1003,11 +918,6 @@
           <t>solar</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1035,11 +945,6 @@
           <t>nasa</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>chinese</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1067,11 +972,6 @@
           <t>material</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>chicken</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1097,11 +997,6 @@
       <c r="E21" t="inlineStr">
         <is>
           <t>fish</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>duck</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added more preprocessing to hw8
</commit_message>
<xml_diff>
--- a/hw8/LSA_group_3.xlsx
+++ b/hw8/LSA_group_3.xlsx
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>belt</t>
+          <t>pun</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>play</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ak</t>
+          <t>confusedsupuerhwomani</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>team</t>
+          <t>cnn</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>best</t>
+          <t>noodle</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -517,12 +517,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>boolongthis</t>
+          <t>pianist</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>play</t>
+          <t>team</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>noodle</t>
+          <t>pork</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,12 +544,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>youempire</t>
+          <t>rosehipskarmamile</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>asteroid</t>
+          <t>player</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -559,24 +559,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>pork</t>
+          <t>rice</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>osiris</t>
+          <t>capsule</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>pianist</t>
+          <t>beatz</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>sample</t>
+          <t>ad</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -586,24 +586,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>rice</t>
+          <t>one</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>rex</t>
+          <t>osirisrex</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>songwriter</t>
+          <t>darjeeling</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>game</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -613,24 +613,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>one</t>
+          <t>best</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>capsule</t>
+          <t>spacecraft</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>earl</t>
+          <t>ringtone</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>player</t>
+          <t>year</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -645,19 +645,19 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dish</t>
+          <t>mission</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ringtone</t>
+          <t>songwriter</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>season</t>
+          <t>game</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -667,12 +667,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>make</t>
+          <t>chinese</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>spacecraft</t>
+          <t>space</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>earth</t>
+          <t>us</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -699,19 +699,19 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>space</t>
+          <t>bennu</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>mindgreenage</t>
+          <t>ak</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>get</t>
+          <t>video</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -726,34 +726,34 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>mission</t>
+          <t>system</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>honey</t>
+          <t>examiner</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>cnn</t>
+          <t>league</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>us</t>
+          <t>country</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>recipe</t>
+          <t>make</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>bennu</t>
+          <t>solar</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>league</t>
+          <t>season</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -775,46 +775,46 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>chinese</t>
+          <t>soup</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>pork</t>
+          <t>nasa</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>swizz</t>
+          <t>bee</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>golf</t>
+          <t>get</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>company</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>duck</t>
+          <t>serve</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>noodle</t>
+          <t>collect</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>alsofiled</t>
+          <t>tmz</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -824,17 +824,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>company</t>
+          <t>us</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>serve</t>
+          <t>duck</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>rice</t>
+          <t>material</t>
         </is>
       </c>
     </row>
@@ -846,39 +846,39 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ad</t>
+          <t>asteroid</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>chip</t>
+          <t>log</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>soup</t>
+          <t>recipe</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>system</t>
+          <t>rock</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>pun</t>
+          <t>earl</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>sample</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>business</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -888,41 +888,41 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>chinese</t>
+          <t>scientist</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2019and</t>
+          <t>honey</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>osiris</t>
+          <t>feedback</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>play</t>
+          <t>chip</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>brownie</t>
+          <t>dan</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>solar</t>
+          <t>planet</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>womani</t>
+          <t>affairlovin</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -932,61 +932,61 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>world</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>fried</t>
+          <t>steam</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>nasa</t>
+          <t>mile</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>examiner</t>
+          <t>empuerh</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>time</t>
+          <t>export</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>tv</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>many</t>
+          <t>sweet</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>material</t>
+          <t>deliver</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>rosehipskarmamile</t>
+          <t>mindgreenage</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>space</t>
+          <t>last</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>tv</t>
+          <t>gallium</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>fish</t>
+          <t>orbit</t>
         </is>
       </c>
     </row>

</xml_diff>